<commit_message>
Comments on sorting AppliedArea
 Added thoughts and potential solutions for sorting the appliedArea polygons list, as well as how to consolidate the list.
</commit_message>
<xml_diff>
--- a/Nozzle Width Calculations (2018.04.19).xlsx
+++ b/Nozzle Width Calculations (2018.04.19).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="10">
   <si>
     <t>dist btwn nozzles</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>Viable combinations (no gaps)</t>
+  </si>
+  <si>
+    <t>2^x</t>
+  </si>
+  <si>
+    <t>x^2</t>
   </si>
 </sst>
 </file>
@@ -476,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:L23"/>
+  <dimension ref="E3:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16:T24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,10 +496,10 @@
     <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -499,7 +508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -507,16 +516,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="L6">
+    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="M6">
         <f>6*F7</f>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,15 +534,16 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="5:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E10" t="str">
         <f t="shared" ref="E10:E23" si="0">IF(F10&lt;($F$4/2),IF(F10=(($F$4-1)/2),"center","left"),IF(AND(F10&lt;&gt;($F$4/2),F10&lt;&gt;""),"right",""))</f>
         <v>left</v>
@@ -548,6 +558,12 @@
         <v>6</v>
       </c>
       <c r="J10">
+        <f>IF(ISEVEN($F$4),
+(($F$4/2)-F10),
+(($F$4-1)/2-F10))</f>
+        <v>6</v>
+      </c>
+      <c r="K10">
         <f>IF(AND(ISEVEN($F$4),I10&gt;0),
 ($F$7/2)+((I10-1)*$F$7),
 IF(ISODD($F$4),
@@ -555,14 +571,14 @@
 0))</f>
         <v>8</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f>IF(AND(ISEVEN($F$4),ABS(($F$4/2)-F10)&gt;0),
 ($F$7/2)+((ABS(($F$4/2)-F10)-1)*$F$7),
 (ABS(($F$4/2)-F10)*$F$7))</f>
         <v>8.6666666666666661</v>
       </c>
     </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
@@ -578,27 +594,33 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J23" si="2">IF(AND(ISEVEN($F$4),I11&gt;0),
+        <f t="shared" ref="J11:J23" si="2">IF(ISEVEN($F$4),
+(($F$4/2)-F11),
+(($F$4-1)/2-F11))</f>
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K23" si="3">IF(AND(ISEVEN($F$4),I11&gt;0),
 ($F$7/2)+((I11-1)*$F$7),
 IF(ISODD($F$4),
 (I11*$F$7),
 0))</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="L11">
-        <f t="shared" ref="L11:L23" si="3">IF(AND(ISEVEN($F$4),ABS(($F$4/2)-F11)&gt;0),
+      <c r="M11">
+        <f t="shared" ref="M11:M23" si="4">IF(AND(ISEVEN($F$4),ABS(($F$4/2)-F11)&gt;0),
 ($F$7/2)+((ABS(($F$4/2)-F11)-1)*$F$7),
 (ABS(($F$4/2)-F11)*$F$7))</f>
         <v>7.333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F23" si="4">IF(ISEVEN($F$4),IF(F11+1&lt;=$F$4,F11+1,""),IF(F11+1&lt;$F$4,F11+1,""))</f>
+        <f t="shared" ref="F12:F23" si="5">IF(ISEVEN($F$4),IF(F11+1&lt;=$F$4,F11+1,""),IF(F11+1&lt;$F$4,F11+1,""))</f>
         <v>2</v>
       </c>
       <c r="I12">
@@ -607,20 +629,24 @@
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
+      <c r="M12">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I13">
@@ -629,20 +655,24 @@
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
+      <c r="M13">
+        <f t="shared" si="4"/>
         <v>4.6666666666666661</v>
       </c>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I14">
@@ -651,20 +681,24 @@
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
+      <c r="M14">
+        <f t="shared" si="4"/>
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I15">
@@ -673,20 +707,24 @@
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
+      <c r="M15">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>center</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I16">
@@ -697,18 +735,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="I17">
@@ -717,20 +759,24 @@
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="3"/>
+      <c r="M17">
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I18">
@@ -739,20 +785,24 @@
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
+      <c r="M18">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="I19">
@@ -761,20 +811,24 @@
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="3"/>
+      <c r="M19">
+        <f t="shared" si="4"/>
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="I20">
@@ -783,20 +837,24 @@
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="3"/>
+      <c r="M20">
+        <f t="shared" si="4"/>
         <v>4.6666666666666661</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="I21">
@@ -805,20 +863,24 @@
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="3"/>
+      <c r="M21">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>right</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="I22">
@@ -827,20 +889,24 @@
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
+      <c r="M22">
+        <f t="shared" si="4"/>
         <v>7.333333333333333</v>
       </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I23" t="e">
@@ -851,8 +917,12 @@
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L23" t="e">
-        <f t="shared" si="3"/>
+      <c r="K23" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" t="e">
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -863,10 +933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM92"/>
+  <dimension ref="A1:AK92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL8" sqref="AL8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,10 +960,13 @@
     <col min="26" max="30" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="2" style="3" customWidth="1"/>
     <col min="32" max="32" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.88671875" style="3"/>
+    <col min="33" max="34" width="8.88671875" style="3"/>
+    <col min="35" max="35" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.6640625" style="3" customWidth="1"/>
+    <col min="37" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -982,7 +1055,7 @@
         <v>______</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1010,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="4" t="str">
-        <f t="shared" ref="K2:K8" si="1">CONCATENATE(IF(ISBLANK(H2),"_",H2),IF(ISBLANK(I2),"_",I2),IF(ISBLANK(J2),"_",J2))</f>
+        <f t="shared" ref="K2:K4" si="1">CONCATENATE(IF(ISBLANK(H2),"_",H2),IF(ISBLANK(I2),"_",I2),IF(ISBLANK(J2),"_",J2))</f>
         <v>xxx</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1067,11 +1140,11 @@
         <v>5</v>
       </c>
       <c r="AF2" s="4" t="str">
-        <f t="shared" ref="AF2:AF65" si="4">CONCATENATE(IF(ISBLANK(Z2),"_",Z2),IF(ISBLANK(AA2),"_",AA2),IF(ISBLANK(AB2),"_",AB2),IF(ISBLANK(AC2),"_",AC2),IF(ISBLANK(AD2),"_",AD2),IF(ISBLANK(AE2),"_",AE2))</f>
+        <f t="shared" ref="AF2:AF64" si="4">CONCATENATE(IF(ISBLANK(Z2),"_",Z2),IF(ISBLANK(AA2),"_",AA2),IF(ISBLANK(AB2),"_",AB2),IF(ISBLANK(AC2),"_",AC2),IF(ISBLANK(AD2),"_",AD2),IF(ISBLANK(AE2),"_",AE2))</f>
         <v>xxxxxx</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1138,7 +1211,7 @@
         <v>xxxxx_</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1205,7 +1278,7 @@
         <v>_xxxxx</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1253,7 +1326,7 @@
         <v>xxxx__</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="I6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1300,8 +1373,17 @@
         <f t="shared" si="4"/>
         <v>_xxxx_</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AI6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1348,14 +1430,22 @@
         <f t="shared" si="4"/>
         <v>__xxxx</v>
       </c>
+      <c r="AH7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>2</v>
+      </c>
       <c r="AJ7" s="3">
+        <f>AH7^2</f>
         <v>1</v>
       </c>
       <c r="AK7" s="3">
+        <f>2^AH7</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="H8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1396,18 +1486,22 @@
         <f t="shared" si="4"/>
         <v>xxx___</v>
       </c>
+      <c r="AH8" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>4</v>
+      </c>
       <c r="AJ8" s="3">
-        <v>2</v>
+        <f t="shared" ref="AJ8:AJ18" si="5">AH8^2</f>
+        <v>4</v>
       </c>
       <c r="AK8" s="3">
+        <f t="shared" ref="AK8:AK18" si="6">2^AH8</f>
         <v>4</v>
       </c>
-      <c r="AM8" s="3">
-        <f t="shared" ref="AM8:AM11" si="5">AK8-AK7</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1438,18 +1532,22 @@
         <f t="shared" si="4"/>
         <v>_xxx__</v>
       </c>
+      <c r="AH9" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>7</v>
+      </c>
       <c r="AJ9" s="3">
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="AK9" s="3">
-        <v>7</v>
-      </c>
-      <c r="AM9" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -1487,18 +1585,22 @@
         <f t="shared" si="4"/>
         <v>__xxx_</v>
       </c>
+      <c r="AH10" s="3">
+        <v>4</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>11</v>
+      </c>
       <c r="AJ10" s="3">
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="AK10" s="3">
-        <v>11</v>
-      </c>
-      <c r="AM10" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="P11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1529,18 +1631,22 @@
         <f t="shared" si="4"/>
         <v>___xxx</v>
       </c>
+      <c r="AH11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>16</v>
+      </c>
       <c r="AJ11" s="3">
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="AK11" s="3">
-        <v>16</v>
-      </c>
-      <c r="AM11" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -1579,18 +1685,22 @@
         <f t="shared" si="4"/>
         <v>xx____</v>
       </c>
+      <c r="AH12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>22</v>
+      </c>
       <c r="AJ12" s="3">
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>36</v>
       </c>
       <c r="AK12" s="3">
-        <v>22</v>
-      </c>
-      <c r="AM12" s="3">
-        <f>AK12-AK11</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <f>IF(A12+1&lt;=$A$10,A12+1,"")</f>
         <v>1</v>
@@ -1600,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13:D76" si="6">2^A13</f>
+        <f t="shared" ref="D13:D76" si="7">2^A13</f>
         <v>2</v>
       </c>
       <c r="N13" s="3" t="s">
@@ -1630,19 +1740,23 @@
         <f t="shared" si="4"/>
         <v>_xx___</v>
       </c>
+      <c r="AH13" s="3">
+        <v>7</v>
+      </c>
+      <c r="AI13" s="3">
+        <f>AI12+AH13</f>
+        <v>29</v>
+      </c>
       <c r="AJ13" s="3">
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>49</v>
       </c>
       <c r="AK13" s="3">
-        <f>AK12+AJ13</f>
-        <v>29</v>
-      </c>
-      <c r="AM13" s="3">
-        <f>AK13-AK12</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <f>IF(A13+1&lt;=$A$10,A13+1,"")</f>
         <v>2</v>
@@ -1652,7 +1766,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="M14" s="3" t="s">
@@ -1682,15 +1796,23 @@
         <f t="shared" si="4"/>
         <v>__xx__</v>
       </c>
+      <c r="AH14" s="3">
+        <v>8</v>
+      </c>
+      <c r="AI14" s="3">
+        <f>AI13+AH14</f>
+        <v>37</v>
+      </c>
       <c r="AJ14" s="3">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>64</v>
       </c>
       <c r="AK14" s="3">
-        <f t="shared" ref="AK14:AK15" si="7">AK13+AJ14</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <f>IF(A14+1&lt;=$A$10,A14+1,"")</f>
         <v>3</v>
@@ -1700,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="M15" s="3" t="s">
@@ -1733,15 +1855,23 @@
         <f t="shared" si="4"/>
         <v>___xx_</v>
       </c>
+      <c r="AH15" s="3">
+        <v>9</v>
+      </c>
+      <c r="AI15" s="3">
+        <f>AI14+AH15</f>
+        <v>46</v>
+      </c>
       <c r="AJ15" s="3">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>81</v>
       </c>
       <c r="AK15" s="3">
-        <f t="shared" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <f>IF(A15+1&lt;=$A$10,A15+1,"")</f>
         <v>4</v>
@@ -1751,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="M16" s="3" t="s">
@@ -1784,8 +1914,23 @@
         <f t="shared" si="4"/>
         <v>____xx</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH16" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI16" s="3">
+        <f>AI15+AH16</f>
+        <v>56</v>
+      </c>
+      <c r="AJ16" s="3">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="AK16" s="3">
+        <f t="shared" si="6"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <f>IF(A16+1&lt;=$A$10,A16+1,"")</f>
         <v>5</v>
@@ -1795,34 +1940,49 @@
         <v>1</v>
       </c>
       <c r="D17" s="3">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X17" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>x_xxx</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>x_____</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>11</v>
+      </c>
+      <c r="AI17" s="3">
+        <f>AI16+AH17</f>
+        <v>67</v>
+      </c>
+      <c r="AJ17" s="3">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="AK17" s="3">
         <f t="shared" si="6"/>
-        <v>32</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X17" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>x_xxx</v>
-      </c>
-      <c r="Z17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF17" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>x_____</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="str">
         <f>IF(A17+1&lt;=$A$10,A17+1,"")</f>
         <v/>
@@ -1832,31 +1992,46 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X18" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>x__xx</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>_x____</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>12</v>
+      </c>
+      <c r="AI18" s="3">
+        <f>AI17+AH18</f>
+        <v>79</v>
+      </c>
+      <c r="AJ18" s="3">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="AK18" s="3">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="W18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X18" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>x__xx</v>
-      </c>
-      <c r="AA18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF18" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>_x____</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="e">
         <f>IF(A18+1&lt;=$A$10,A18+1,"")</f>
         <v>#VALUE!</v>
@@ -1866,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S19" s="3" t="s">
@@ -1887,7 +2062,7 @@
         <v>__x___</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="e">
         <f>IF(A19+1&lt;=$A$10,A19+1,"")</f>
         <v>#VALUE!</v>
@@ -1897,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S20" s="3" t="s">
@@ -1921,7 +2096,7 @@
         <v>___x__</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="e">
         <f>IF(A20+1&lt;=$A$10,A20+1,"")</f>
         <v>#VALUE!</v>
@@ -1931,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -1952,7 +2127,7 @@
         <v>____x_</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="e">
         <f>IF(A21+1&lt;=$A$10,A21+1,"")</f>
         <v>#VALUE!</v>
@@ -1962,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S22" s="3" t="s">
@@ -1983,7 +2158,7 @@
         <v>_____x</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="e">
         <f>IF(A22+1&lt;=$A$10,A22+1,"")</f>
         <v>#VALUE!</v>
@@ -1993,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S23" s="3" t="s">
@@ -2029,7 +2204,7 @@
         <v>x_xxxx</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="e">
         <f>IF(A23+1&lt;=$A$10,A23+1,"")</f>
         <v>#VALUE!</v>
@@ -2039,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S24" s="3" t="s">
@@ -2072,7 +2247,7 @@
         <v>x__xxx</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="e">
         <f>IF(A24+1&lt;=$A$10,A24+1,"")</f>
         <v>#VALUE!</v>
@@ -2082,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -2115,7 +2290,7 @@
         <v>x___xx</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="e">
         <f>IF(A25+1&lt;=$A$10,A25+1,"")</f>
         <v>#VALUE!</v>
@@ -2125,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S26" s="3" t="s">
@@ -2161,7 +2336,7 @@
         <v>xx_xxx</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="e">
         <f>IF(A26+1&lt;=$A$10,A26+1,"")</f>
         <v>#VALUE!</v>
@@ -2171,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="T27" s="3" t="s">
@@ -2207,7 +2382,7 @@
         <v>xxx_xx</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="e">
         <f>IF(A27+1&lt;=$A$10,A27+1,"")</f>
         <v>#VALUE!</v>
@@ -2217,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="U28" s="3" t="s">
@@ -2250,7 +2425,7 @@
         <v>xxxx_x</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="e">
         <f>IF(A28+1&lt;=$A$10,A28+1,"")</f>
         <v>#VALUE!</v>
@@ -2260,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="S29" s="3" t="s">
@@ -2296,7 +2471,7 @@
         <v>xx__xx</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="e">
         <f>IF(A29+1&lt;=$A$10,A29+1,"")</f>
         <v>#VALUE!</v>
@@ -2306,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="T30" s="3" t="s">
@@ -2336,7 +2511,7 @@
         <v>xx_x_x</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="e">
         <f>IF(A30+1&lt;=$A$10,A30+1,"")</f>
         <v>#VALUE!</v>
@@ -2346,7 +2521,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="T31" s="3" t="s">
@@ -2379,7 +2554,7 @@
         <v>_x_xxx</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="e">
         <f>IF(A31+1&lt;=$A$10,A31+1,"")</f>
         <v>#VALUE!</v>
@@ -2389,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="T32" s="3" t="s">
@@ -2426,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA33" s="3" t="s">
@@ -2450,7 +2625,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB34" s="3" t="s">
@@ -2474,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC35" s="3" t="s">
@@ -2498,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA36" s="3" t="s">
@@ -2525,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA37" s="3" t="s">
@@ -2555,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z38" s="3" t="s">
@@ -2585,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z39" s="3" t="s">
@@ -2612,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z40" s="3" t="s">
@@ -2642,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB41" s="3" t="s">
@@ -2669,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB42" s="3" t="s">
@@ -2696,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA43" s="3" t="s">
@@ -2726,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA44" s="3" t="s">
@@ -2753,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z45" s="3" t="s">
@@ -2783,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z46" s="3" t="s">
@@ -2810,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z47" s="3" t="s">
@@ -2840,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z48" s="3" t="s">
@@ -2867,7 +3042,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z49" s="3" t="s">
@@ -2891,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z50" s="3" t="s">
@@ -2918,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z51" s="3" t="s">
@@ -2942,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z52" s="3" t="s">
@@ -2966,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="D53" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z53" s="3" t="s">
@@ -2993,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="D54" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z54" s="3" t="s">
@@ -3020,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z55" s="3" t="s">
@@ -3050,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z56" s="3" t="s">
@@ -3077,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA57" s="3" t="s">
@@ -3104,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="D58" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB58" s="3" t="s">
@@ -3128,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z59" s="3" t="s">
@@ -3158,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA60" s="3" t="s">
@@ -3182,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="D61" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA61" s="3" t="s">
@@ -3209,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="D62" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="AA62" s="3" t="s">
@@ -3233,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="D63" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z63" s="3" t="s">
@@ -3257,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z64" s="3" t="s">
@@ -3284,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3298,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3312,7 +3487,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3326,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3340,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3354,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="D70" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3368,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3382,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="D72" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3396,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="D73" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3410,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3424,7 +3599,7 @@
         <v>0</v>
       </c>
       <c r="D75" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3438,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="D76" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>